<commit_message>
Library management system added
</commit_message>
<xml_diff>
--- a/working/Learning Summary.xlsx
+++ b/working/Learning Summary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t>join,inner join,outer join,first,firstDefualt,dependency injection,single,singledefault,authorization,authentication.</t>
+  </si>
+  <si>
+    <t>depencency injection method=&gt;constructor,property,function,webapi completed with database connection ,migration ,code first,db first approach.</t>
+  </si>
+  <si>
+    <t>web api using dbfirst approach ,data table created for the project,lms api project category post and books get,post api</t>
+  </si>
+  <si>
+    <t>LibraryMgmtSystem project addbook,user,category,borrow record =&gt;post,get api controller completed</t>
   </si>
 </sst>
 </file>
@@ -417,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,6 +594,30 @@
         <v>24</v>
       </c>
     </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>45497</v>
+      </c>
+      <c r="C34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>45498</v>
+      </c>
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>45499</v>
+      </c>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>